<commit_message>
Consistency of deviations plots finished
</commit_message>
<xml_diff>
--- a/3scenarios/telemetry/DeviationsTable_Traditional.xlsx
+++ b/3scenarios/telemetry/DeviationsTable_Traditional.xlsx
@@ -8,13 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Deviations" sheetId="1" r:id="rId1"/>
+    <sheet name="CountVsDeviation" sheetId="2" r:id="rId2"/>
+    <sheet name="CountVsDeviation_t" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>1</t>
   </si>
@@ -47,6 +49,63 @@
   </si>
   <si>
     <t>Scenario Average</t>
+  </si>
+  <si>
+    <t>Scenario Max</t>
+  </si>
+  <si>
+    <t>deviation intervals</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>0.43-0.59</t>
+  </si>
+  <si>
+    <t>0.59-0.74</t>
+  </si>
+  <si>
+    <t>0.74-0.9</t>
+  </si>
+  <si>
+    <t>0.9-1.05</t>
+  </si>
+  <si>
+    <t>1.05-1.21</t>
+  </si>
+  <si>
+    <t>1.21-1.37</t>
+  </si>
+  <si>
+    <t>1.37-1.52</t>
+  </si>
+  <si>
+    <t>1.52-1.68</t>
+  </si>
+  <si>
+    <t>1.68-1.84</t>
+  </si>
+  <si>
+    <t>1.84-1.99</t>
+  </si>
+  <si>
+    <t>1.99-2.15</t>
+  </si>
+  <si>
+    <t>2.15-2.3</t>
+  </si>
+  <si>
+    <t>2.3-2.46</t>
+  </si>
+  <si>
+    <t>2.46-2.62</t>
+  </si>
+  <si>
+    <t>2.62-2.77</t>
+  </si>
+  <si>
+    <t>2.77-2.93</t>
   </si>
 </sst>
 </file>
@@ -117,6 +176,951 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" baseline="0">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Count vs Mean Deviation
+PI(t)D(t) All Scenarios</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.089999999999999997"/>
+          <c:y val="0.20000000000000001"/>
+          <c:w val="0.87"/>
+          <c:h val="0.5"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="BF0000"/>
+            </a:solidFill>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>CountVsDeviation!$B$2:$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.43-0.59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59-0.74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.74-0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9-1.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.05-1.21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.21-1.37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.37-1.52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.52-1.68</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.68-1.84</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.84-1.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.99-2.15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.15-2.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3-2.46</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.46-2.62</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.62-2.77</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.77-2.93</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CountVsDeviation!$C$2:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:srgbClr val="700000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="700000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="700000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>CountVsDeviation!$B$2:$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.43-0.59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59-0.74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.74-0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9-1.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.05-1.21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.21-1.37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.37-1.52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.52-1.68</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.68-1.84</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.84-1.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.99-2.15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.15-2.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3-2.46</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.46-2.62</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.62-2.77</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.77-2.93</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CountVsDeviation!$C$2:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50010001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" baseline="0">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Trial Mean Deviation from Target Path (in)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" baseline="0">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="50010002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50010002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="16"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" baseline="0">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" baseline="0">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="50010001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" baseline="0">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Count vs Mean Deviation
+PID All Scenarios</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.089999999999999997"/>
+          <c:y val="0.20000000000000001"/>
+          <c:w val="0.87"/>
+          <c:h val="0.5"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>CountVsDeviation_t!$B$2:$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.43-0.59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59-0.74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.74-0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9-1.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.05-1.21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.21-1.37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.37-1.52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.52-1.68</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.68-1.84</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.84-1.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.99-2.15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.15-2.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3-2.46</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.46-2.62</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.62-2.77</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.77-2.93</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CountVsDeviation_t!$C$2:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50020001"/>
+        <c:axId val="50020002"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:srgbClr val="00306B"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00306B"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="00306B"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>CountVsDeviation_t!$B$2:$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.43-0.59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59-0.74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.74-0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9-1.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.05-1.21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.21-1.37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.37-1.52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.52-1.68</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.68-1.84</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.84-1.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.99-2.15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.15-2.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3-2.46</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.46-2.62</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.62-2.77</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.77-2.93</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CountVsDeviation_t!$C$2:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50020001"/>
+        <c:axId val="50020002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50020001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" baseline="0">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Trial Mean Deviation from Target Path (in)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" baseline="0">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="50020002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50020002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="16"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" baseline="0">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" baseline="0">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="50020001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -404,13 +1408,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,8 +1448,11 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -482,8 +1489,11 @@
       <c r="L2">
         <v>1.823</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2">
+        <v>4.401</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -520,8 +1530,11 @@
       <c r="L3">
         <v>1.656</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3">
+        <v>3.493</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -558,8 +1571,11 @@
       <c r="L4">
         <v>2.444</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4">
+        <v>10.483</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -596,8 +1612,11 @@
       <c r="L5">
         <v>1.551</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -634,8 +1653,11 @@
       <c r="L6">
         <v>0.961</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6">
+        <v>2.601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -671,9 +1693,408 @@
       </c>
       <c r="L7">
         <v>1.561</v>
+      </c>
+      <c r="M7">
+        <v>7.042</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
formatted mean avg deviations table in excel
</commit_message>
<xml_diff>
--- a/3scenarios/telemetry/DeviationsTable_Traditional.xlsx
+++ b/3scenarios/telemetry/DeviationsTable_Traditional.xlsx
@@ -1,58 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael_Zeng\Documents\VAMP - Science Fair 2021\Python Plotting\3scenarios\telemetry\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA519576-DEC6-4C13-9792-799DA0DA21A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Deviations" sheetId="1" r:id="rId1"/>
-    <sheet name="CountVsDeviation" sheetId="2" r:id="rId2"/>
-    <sheet name="CountVsDeviation_t" sheetId="3" r:id="rId3"/>
+    <sheet name="Max Errors" sheetId="4" r:id="rId2"/>
+    <sheet name="CountVsDeviation" sheetId="2" r:id="rId3"/>
+    <sheet name="CountVsDeviation_t" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Scenario Average</t>
-  </si>
-  <si>
-    <t>Scenario Max</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t>deviation intervals</t>
   </si>
@@ -106,13 +77,82 @@
   </si>
   <si>
     <t>2.77-2.93</t>
+  </si>
+  <si>
+    <t>Trial 1</t>
+  </si>
+  <si>
+    <t>Trial 2</t>
+  </si>
+  <si>
+    <t>Trial 3</t>
+  </si>
+  <si>
+    <t>Trial 4</t>
+  </si>
+  <si>
+    <t>Trial 5</t>
+  </si>
+  <si>
+    <t>Trial 6</t>
+  </si>
+  <si>
+    <t>Trial 7</t>
+  </si>
+  <si>
+    <t>Trial 8</t>
+  </si>
+  <si>
+    <t>Trial 9</t>
+  </si>
+  <si>
+    <t>Trial 10</t>
+  </si>
+  <si>
+    <t>PI(t)D(t)</t>
+  </si>
+  <si>
+    <t>Traditional PID</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
+    <t>Mean Average Deviation From Target Path (in)</t>
+  </si>
+  <si>
+    <t>Average of 10 Trials</t>
+  </si>
+  <si>
+    <t>Max.</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>Scenario 1</t>
+  </si>
+  <si>
+    <t>Scenario 2</t>
+  </si>
+  <si>
+    <t>Scenario 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +167,32 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,10 +230,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -175,12 +263,30 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -203,16 +309,17 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.089999999999999997"/>
-          <c:y val="0.20000000000000001"/>
+          <c:x val="0.09"/>
+          <c:y val="0.2"/>
           <c:w val="0.87"/>
           <c:h val="0.5"/>
         </c:manualLayout>
@@ -220,6 +327,7 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -233,6 +341,7 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>CountVsDeviation!$B$2:$B$17</c:f>
@@ -346,12 +455,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0C9D-4E44-8DB2-2E7296B1CD00}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="50010001"/>
         <c:axId val="50010002"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -364,6 +488,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="diamond"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="700000"/>
@@ -489,8 +614,22 @@
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0C9D-4E44-8DB2-2E7296B1CD00}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="50010001"/>
         <c:axId val="50010002"/>
       </c:lineChart>
@@ -499,6 +638,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -520,9 +660,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="19050">
@@ -548,6 +690,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50010002"/>
@@ -556,6 +699,7 @@
           <c:max val="16"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -577,7 +721,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
@@ -608,6 +752,8 @@
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -618,8 +764,18 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -642,16 +798,17 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.089999999999999997"/>
-          <c:y val="0.20000000000000001"/>
+          <c:x val="0.09"/>
+          <c:y val="0.2"/>
           <c:w val="0.87"/>
           <c:h val="0.5"/>
         </c:manualLayout>
@@ -659,6 +816,7 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -669,6 +827,7 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>CountVsDeviation_t!$B$2:$B$17</c:f>
@@ -782,12 +941,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6A4A-4B58-A0D1-8F237D878DF7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="50020001"/>
         <c:axId val="50020002"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -800,6 +974,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="diamond"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00306B"/>
@@ -925,8 +1100,22 @@
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6A4A-4B58-A0D1-8F237D878DF7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="50020001"/>
         <c:axId val="50020002"/>
       </c:lineChart>
@@ -935,6 +1124,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -956,9 +1146,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="19050">
@@ -984,6 +1176,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50020002"/>
@@ -992,6 +1185,7 @@
           <c:max val="16"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -1013,7 +1207,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
@@ -1044,6 +1238,8 @@
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1070,7 +1266,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1105,7 +1307,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1166,7 +1374,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1198,9 +1406,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1232,6 +1458,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1407,489 +1651,608 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="12.29296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10" style="3" customWidth="1"/>
+    <col min="3" max="12" width="8.9375" style="3"/>
+    <col min="13" max="13" width="18.52734375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.5859375" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="8.9375" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="11">
         <v>1.865</v>
       </c>
-      <c r="C2">
-        <v>1.777</v>
-      </c>
-      <c r="D2">
+      <c r="D4" s="11">
+        <v>1.7769999999999999</v>
+      </c>
+      <c r="E4" s="11">
         <v>1.819</v>
       </c>
-      <c r="E2">
-        <v>1.769</v>
-      </c>
-      <c r="F2">
+      <c r="F4" s="11">
+        <v>1.7689999999999999</v>
+      </c>
+      <c r="G4" s="11">
         <v>1.637</v>
       </c>
-      <c r="G2">
-        <v>1.933</v>
-      </c>
-      <c r="H2">
+      <c r="H4" s="11">
+        <v>1.9330000000000001</v>
+      </c>
+      <c r="I4" s="11">
         <v>1.92</v>
       </c>
-      <c r="I2">
-        <v>1.733</v>
-      </c>
-      <c r="J2">
-        <v>1.874</v>
-      </c>
-      <c r="K2">
-        <v>1.908</v>
-      </c>
-      <c r="L2">
+      <c r="J4" s="11">
+        <v>1.7330000000000001</v>
+      </c>
+      <c r="K4" s="11">
+        <v>1.8740000000000001</v>
+      </c>
+      <c r="L4" s="11">
+        <v>1.9079999999999999</v>
+      </c>
+      <c r="M4" s="11">
         <v>1.823</v>
       </c>
-      <c r="M2">
-        <v>4.401</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A5" s="6"/>
+      <c r="B5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="11">
         <v>1.556</v>
       </c>
-      <c r="C3">
+      <c r="D5" s="11">
         <v>1.536</v>
       </c>
-      <c r="D3">
+      <c r="E5" s="11">
         <v>1.679</v>
       </c>
-      <c r="E3">
-        <v>1.685</v>
-      </c>
-      <c r="F3">
+      <c r="F5" s="11">
+        <v>1.6850000000000001</v>
+      </c>
+      <c r="G5" s="11">
         <v>1.54</v>
       </c>
-      <c r="G3">
+      <c r="H5" s="11">
         <v>1.7</v>
       </c>
-      <c r="H3">
-        <v>1.539</v>
-      </c>
-      <c r="I3">
+      <c r="I5" s="11">
+        <v>1.5389999999999999</v>
+      </c>
+      <c r="J5" s="11">
         <v>1.774</v>
       </c>
-      <c r="J3">
-        <v>1.813</v>
-      </c>
-      <c r="K3">
+      <c r="K5" s="11">
+        <v>1.8129999999999999</v>
+      </c>
+      <c r="L5" s="11">
         <v>1.74</v>
       </c>
-      <c r="L3">
-        <v>1.656</v>
-      </c>
-      <c r="M3">
-        <v>3.493</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
+      <c r="M5" s="11">
+        <v>1.6559999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A6" s="6"/>
+      <c r="B6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="11">
         <v>2.379</v>
       </c>
-      <c r="C4">
-        <v>2.352</v>
-      </c>
-      <c r="D4">
-        <v>2.332</v>
-      </c>
-      <c r="E4">
-        <v>2.592</v>
-      </c>
-      <c r="F4">
-        <v>2.365</v>
-      </c>
-      <c r="G4">
-        <v>2.364</v>
-      </c>
-      <c r="H4">
+      <c r="D6" s="11">
+        <v>2.3519999999999999</v>
+      </c>
+      <c r="E6" s="11">
+        <v>2.3319999999999999</v>
+      </c>
+      <c r="F6" s="11">
+        <v>2.5920000000000001</v>
+      </c>
+      <c r="G6" s="11">
+        <v>2.3650000000000002</v>
+      </c>
+      <c r="H6" s="11">
+        <v>2.3639999999999999</v>
+      </c>
+      <c r="I6" s="11">
         <v>2.65</v>
       </c>
-      <c r="I4">
-        <v>2.396</v>
-      </c>
-      <c r="J4">
-        <v>2.563</v>
-      </c>
-      <c r="K4">
+      <c r="J6" s="11">
+        <v>2.3959999999999999</v>
+      </c>
+      <c r="K6" s="11">
+        <v>2.5630000000000002</v>
+      </c>
+      <c r="L6" s="11">
         <v>2.444</v>
       </c>
-      <c r="L4">
+      <c r="M6" s="11">
         <v>2.444</v>
       </c>
-      <c r="M4">
-        <v>10.483</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="11">
         <v>1.526</v>
       </c>
-      <c r="C5">
+      <c r="D7" s="11">
         <v>1.61</v>
       </c>
-      <c r="D5">
+      <c r="E7" s="11">
         <v>1.534</v>
       </c>
-      <c r="E5">
+      <c r="F7" s="11">
         <v>1.532</v>
       </c>
-      <c r="F5">
-        <v>1.501</v>
-      </c>
-      <c r="G5">
-        <v>1.566</v>
-      </c>
-      <c r="H5">
-        <v>1.551</v>
-      </c>
-      <c r="I5">
+      <c r="G7" s="11">
+        <v>1.5009999999999999</v>
+      </c>
+      <c r="H7" s="11">
+        <v>1.5660000000000001</v>
+      </c>
+      <c r="I7" s="11">
+        <v>1.5509999999999999</v>
+      </c>
+      <c r="J7" s="11">
         <v>1.581</v>
       </c>
-      <c r="J5">
-        <v>1.511</v>
-      </c>
-      <c r="K5">
+      <c r="K7" s="11">
+        <v>1.5109999999999999</v>
+      </c>
+      <c r="L7" s="11">
         <v>1.599</v>
       </c>
-      <c r="L5">
-        <v>1.551</v>
-      </c>
-      <c r="M5">
+      <c r="M7" s="11">
+        <v>1.5509999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A8" s="7"/>
+      <c r="B8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="E8" s="11">
+        <v>1.0309999999999999</v>
+      </c>
+      <c r="F8" s="11">
+        <v>1.0669999999999999</v>
+      </c>
+      <c r="G8" s="11">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="H8" s="11">
+        <v>1.0920000000000001</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0.97</v>
+      </c>
+      <c r="J8" s="11">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="K8" s="11">
+        <v>0.71</v>
+      </c>
+      <c r="L8" s="11">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="M8" s="11">
+        <v>0.96099999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A9" s="7"/>
+      <c r="B9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="11">
+        <v>1.506</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1.5660000000000001</v>
+      </c>
+      <c r="E9" s="11">
+        <v>1.526</v>
+      </c>
+      <c r="F9" s="11">
+        <v>1.617</v>
+      </c>
+      <c r="G9" s="11">
+        <v>1.52</v>
+      </c>
+      <c r="H9" s="11">
+        <v>1.649</v>
+      </c>
+      <c r="I9" s="11">
+        <v>1.6419999999999999</v>
+      </c>
+      <c r="J9" s="11">
+        <v>1.5029999999999999</v>
+      </c>
+      <c r="K9" s="11">
+        <v>1.5640000000000001</v>
+      </c>
+      <c r="L9" s="11">
+        <v>1.512</v>
+      </c>
+      <c r="M9" s="11">
+        <v>1.5609999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A2:N2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355C86CE-BFB6-43FA-832D-BE0FD0F1F993}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="2" max="2" width="3.52734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="C1" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="5">
+        <v>4.4009999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A3" s="6"/>
+      <c r="B3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="5">
+        <v>3.4929999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="6"/>
+      <c r="B4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="5">
+        <v>10.483000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5">
         <v>3.6</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>0.975</v>
-      </c>
-      <c r="C6">
-        <v>1.003</v>
-      </c>
-      <c r="D6">
-        <v>1.031</v>
-      </c>
-      <c r="E6">
-        <v>1.067</v>
-      </c>
-      <c r="F6">
-        <v>1.001</v>
-      </c>
-      <c r="G6">
-        <v>1.092</v>
-      </c>
-      <c r="H6">
-        <v>0.97</v>
-      </c>
-      <c r="I6">
-        <v>0.916</v>
-      </c>
-      <c r="J6">
-        <v>0.71</v>
-      </c>
-      <c r="K6">
-        <v>0.846</v>
-      </c>
-      <c r="L6">
-        <v>0.961</v>
-      </c>
-      <c r="M6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A6" s="7"/>
+      <c r="B6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="5">
         <v>2.601</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>1.506</v>
-      </c>
-      <c r="C7">
-        <v>1.566</v>
-      </c>
-      <c r="D7">
-        <v>1.526</v>
-      </c>
-      <c r="E7">
-        <v>1.617</v>
-      </c>
-      <c r="F7">
-        <v>1.52</v>
-      </c>
-      <c r="G7">
-        <v>1.649</v>
-      </c>
-      <c r="H7">
-        <v>1.642</v>
-      </c>
-      <c r="I7">
-        <v>1.503</v>
-      </c>
-      <c r="J7">
-        <v>1.564</v>
-      </c>
-      <c r="K7">
-        <v>1.512</v>
-      </c>
-      <c r="L7">
-        <v>1.561</v>
-      </c>
-      <c r="M7">
-        <v>7.042</v>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A7" s="7"/>
+      <c r="B7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="5">
+        <v>7.0419999999999998</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1901,193 +2264,193 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>0</v>

</xml_diff>